<commit_message>
Travis - Reload of GitHub files
</commit_message>
<xml_diff>
--- a/Documents/Expenses.xlsx
+++ b/Documents/Expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>8-tab dividers</t>
+  </si>
+  <si>
+    <t>60 pages printed</t>
   </si>
 </sst>
 </file>
@@ -516,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,13 +662,27 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <v>41688</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
@@ -791,7 +808,7 @@
       <c r="C22" s="11"/>
       <c r="D22" s="9">
         <f>SUM(D4:D21)</f>
-        <v>18.61</v>
+        <v>24.61</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>12</v>
@@ -811,7 +828,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;LUpdated January 26, 2014
+    <oddHeader>&amp;LUpdated February 19, 2014
 &amp;R&amp;P</oddHeader>
   </headerFooter>
 </worksheet>

</xml_diff>